<commit_message>
Sua mensagem de commit
</commit_message>
<xml_diff>
--- a/Base/Backlog.xlsx
+++ b/Base/Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franciscoj\Python_Initial\Pyhton_Web\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04013A9D-4789-41C0-A9DD-8A38295C8A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1288ED45-00EB-4018-9552-3FB2E9BF5A85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{89A3EF9E-2AF9-420D-85DF-9BB5B68F651F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{89A3EF9E-2AF9-420D-85DF-9BB5B68F651F}"/>
   </bookViews>
   <sheets>
     <sheet name="SPN" sheetId="1" r:id="rId1"/>
@@ -168,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -183,6 +183,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,7 +510,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="K26" sqref="K25:L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1362,8 +1372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69362A46-9E44-40AB-81A2-018EE27C1DC6}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1412,291 +1422,291 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="4">
-        <v>45572</v>
-      </c>
-      <c r="E2" s="4">
-        <v>45576</v>
-      </c>
-      <c r="F2" s="1">
+      <c r="C2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="7">
+        <v>45572</v>
+      </c>
+      <c r="E2" s="7">
+        <v>45576</v>
+      </c>
+      <c r="F2" s="6">
         <v>301630</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="8">
         <v>45505</v>
       </c>
-      <c r="H2" s="4">
-        <v>45576</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="H2" s="7">
+        <v>45576</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="4">
-        <v>45572</v>
-      </c>
-      <c r="E3" s="4">
-        <v>45576</v>
-      </c>
-      <c r="F3" s="1">
+      <c r="C3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="7">
+        <v>45572</v>
+      </c>
+      <c r="E3" s="7">
+        <v>45576</v>
+      </c>
+      <c r="F3" s="6">
         <v>303042</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="8">
         <v>45505</v>
       </c>
-      <c r="H3" s="4">
-        <v>45576</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="H3" s="7">
+        <v>45576</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="4">
-        <v>45572</v>
-      </c>
-      <c r="E4" s="4">
-        <v>45576</v>
-      </c>
-      <c r="F4" s="1">
+      <c r="C4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="7">
+        <v>45572</v>
+      </c>
+      <c r="E4" s="7">
+        <v>45576</v>
+      </c>
+      <c r="F4" s="6">
         <v>303197</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="8">
         <v>45505</v>
       </c>
-      <c r="H4" s="4">
-        <v>45576</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" s="1" t="s">
+      <c r="H4" s="7">
+        <v>45576</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="4">
-        <v>45572</v>
-      </c>
-      <c r="E5" s="4">
-        <v>45576</v>
-      </c>
-      <c r="F5" s="1">
+      <c r="C5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="7">
+        <v>45572</v>
+      </c>
+      <c r="E5" s="7">
+        <v>45576</v>
+      </c>
+      <c r="F5" s="6">
         <v>303940</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="8">
         <v>45505</v>
       </c>
-      <c r="H5" s="4">
-        <v>45576</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" s="1" t="s">
+      <c r="H5" s="7">
+        <v>45576</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="4">
-        <v>45572</v>
-      </c>
-      <c r="E6" s="4">
-        <v>45576</v>
-      </c>
-      <c r="F6" s="1">
+      <c r="C6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="7">
+        <v>45572</v>
+      </c>
+      <c r="E6" s="7">
+        <v>45576</v>
+      </c>
+      <c r="F6" s="6">
         <v>303363</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="8">
         <v>45505</v>
       </c>
-      <c r="H6" s="4">
-        <v>45576</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" s="1" t="s">
+      <c r="H6" s="7">
+        <v>45576</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="4">
-        <v>45572</v>
-      </c>
-      <c r="E7" s="4">
-        <v>45576</v>
-      </c>
-      <c r="F7" s="1">
+      <c r="C7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="7">
+        <v>45572</v>
+      </c>
+      <c r="E7" s="7">
+        <v>45576</v>
+      </c>
+      <c r="F7" s="6">
         <v>302085</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="8">
         <v>45505</v>
       </c>
-      <c r="H7" s="4">
-        <v>45576</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" s="1" t="s">
+      <c r="H7" s="7">
+        <v>45576</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="4">
-        <v>45572</v>
-      </c>
-      <c r="E8" s="4">
-        <v>45576</v>
-      </c>
-      <c r="F8" s="1">
+      <c r="C8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="7">
+        <v>45572</v>
+      </c>
+      <c r="E8" s="7">
+        <v>45576</v>
+      </c>
+      <c r="F8" s="6">
         <v>302167</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="8">
         <v>45505</v>
       </c>
-      <c r="H8" s="4">
-        <v>45576</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" s="1" t="s">
+      <c r="H8" s="7">
+        <v>45576</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="4">
-        <v>45572</v>
-      </c>
-      <c r="E9" s="4">
-        <v>45576</v>
-      </c>
-      <c r="F9" s="1">
+      <c r="C9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="7">
+        <v>45572</v>
+      </c>
+      <c r="E9" s="7">
+        <v>45576</v>
+      </c>
+      <c r="F9" s="6">
         <v>303394</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="8">
         <v>45505</v>
       </c>
-      <c r="H9" s="4">
-        <v>45576</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J9" s="1" t="s">
+      <c r="H9" s="7">
+        <v>45576</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="4">
-        <v>45572</v>
-      </c>
-      <c r="E10" s="4">
-        <v>45576</v>
-      </c>
-      <c r="F10" s="1">
+      <c r="C10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="7">
+        <v>45572</v>
+      </c>
+      <c r="E10" s="7">
+        <v>45576</v>
+      </c>
+      <c r="F10" s="6">
         <v>300735</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="8">
         <v>45505</v>
       </c>
-      <c r="H10" s="4">
-        <v>45576</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J10" s="1" t="s">
+      <c r="H10" s="7">
+        <v>45576</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="6" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Mensagem do commit explicando as alterações
</commit_message>
<xml_diff>
--- a/Base/Backlog.xlsx
+++ b/Base/Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franciscoj\Python_Initial\Pyhton_Web\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1288ED45-00EB-4018-9552-3FB2E9BF5A85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067061EB-274F-4B59-B1D8-B3ABF0F11636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{89A3EF9E-2AF9-420D-85DF-9BB5B68F651F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{89A3EF9E-2AF9-420D-85DF-9BB5B68F651F}"/>
   </bookViews>
   <sheets>
     <sheet name="SPN" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="25">
   <si>
     <t>Backlog</t>
   </si>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t>Semana</t>
-  </si>
-  <si>
-    <t>Semana 01</t>
   </si>
   <si>
     <t>Inicio_Semana</t>
@@ -509,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16A6A408-5BF6-4E16-8C71-EC6EB1F5A842}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K26" sqref="K25:L26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,10 +536,10 @@
         <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>1</v>
@@ -557,7 +554,7 @@
         <v>6</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -565,10 +562,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
       </c>
       <c r="D2" s="4">
         <v>45572</v>
@@ -586,10 +583,10 @@
         <v>45576</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -597,10 +594,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
       </c>
       <c r="D3" s="4">
         <v>45572</v>
@@ -618,10 +615,10 @@
         <v>45576</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -629,10 +626,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
       </c>
       <c r="D4" s="4">
         <v>45572</v>
@@ -650,10 +647,10 @@
         <v>45576</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -661,10 +658,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
       </c>
       <c r="D5" s="4">
         <v>45572</v>
@@ -682,10 +679,10 @@
         <v>45576</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -693,10 +690,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
       </c>
       <c r="D6" s="4">
         <v>45572</v>
@@ -714,10 +711,10 @@
         <v>45576</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -725,10 +722,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
       </c>
       <c r="D7" s="4">
         <v>45572</v>
@@ -746,10 +743,10 @@
         <v>45576</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -757,10 +754,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
       </c>
       <c r="D8" s="4">
         <v>45572</v>
@@ -778,10 +775,10 @@
         <v>45576</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -789,10 +786,10 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
       </c>
       <c r="D9" s="4">
         <v>45572</v>
@@ -810,10 +807,10 @@
         <v>45576</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -821,10 +818,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
       </c>
       <c r="D10" s="4">
         <v>45572</v>
@@ -842,10 +839,10 @@
         <v>45576</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -853,10 +850,10 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
       </c>
       <c r="D11" s="4">
         <v>45572</v>
@@ -874,10 +871,10 @@
         <v>45576</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -885,10 +882,10 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
       </c>
       <c r="D12" s="4">
         <v>45572</v>
@@ -906,10 +903,10 @@
         <v>45576</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -917,10 +914,10 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
       </c>
       <c r="D13" s="4">
         <v>45572</v>
@@ -938,10 +935,10 @@
         <v>45576</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -949,10 +946,10 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
       </c>
       <c r="D14" s="4">
         <v>45572</v>
@@ -970,10 +967,10 @@
         <v>45576</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -981,10 +978,10 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
       </c>
       <c r="D15" s="4">
         <v>45572</v>
@@ -1002,10 +999,10 @@
         <v>45576</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1013,10 +1010,10 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
       </c>
       <c r="D16" s="4">
         <v>45572</v>
@@ -1034,10 +1031,10 @@
         <v>45576</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1045,10 +1042,10 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
       </c>
       <c r="D17" s="4">
         <v>45572</v>
@@ -1066,10 +1063,10 @@
         <v>45576</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1077,10 +1074,10 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
       </c>
       <c r="D18" s="4">
         <v>45572</v>
@@ -1098,10 +1095,10 @@
         <v>45576</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1109,10 +1106,10 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
       </c>
       <c r="D19" s="4">
         <v>45572</v>
@@ -1130,10 +1127,10 @@
         <v>45576</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1141,10 +1138,10 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1</v>
       </c>
       <c r="D20" s="4">
         <v>45572</v>
@@ -1162,10 +1159,10 @@
         <v>45576</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1173,10 +1170,10 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
       </c>
       <c r="D21" s="4">
         <v>45572</v>
@@ -1194,10 +1191,10 @@
         <v>45576</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1205,10 +1202,10 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1</v>
       </c>
       <c r="D22" s="4">
         <v>45572</v>
@@ -1226,10 +1223,10 @@
         <v>45576</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1237,10 +1234,10 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1</v>
       </c>
       <c r="D23" s="4">
         <v>45572</v>
@@ -1258,10 +1255,10 @@
         <v>45576</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1269,10 +1266,10 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
       </c>
       <c r="D24" s="4">
         <v>45572</v>
@@ -1290,10 +1287,10 @@
         <v>45576</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1301,10 +1298,10 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1</v>
       </c>
       <c r="D25" s="4">
         <v>45572</v>
@@ -1322,10 +1319,10 @@
         <v>45576</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1333,10 +1330,10 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1</v>
       </c>
       <c r="D26" s="4">
         <v>45572</v>
@@ -1354,10 +1351,10 @@
         <v>45576</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1372,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69362A46-9E44-40AB-81A2-018EE27C1DC6}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1401,10 +1398,10 @@
         <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>1</v>
@@ -1419,7 +1416,7 @@
         <v>6</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1427,10 +1424,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>9</v>
+        <v>20</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
       </c>
       <c r="D2" s="7">
         <v>45572</v>
@@ -1448,10 +1445,10 @@
         <v>45576</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1459,10 +1456,10 @@
         <v>5</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>9</v>
+        <v>20</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
       </c>
       <c r="D3" s="7">
         <v>45572</v>
@@ -1480,10 +1477,10 @@
         <v>45576</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1491,10 +1488,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>9</v>
+        <v>20</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
       </c>
       <c r="D4" s="7">
         <v>45572</v>
@@ -1512,10 +1509,10 @@
         <v>45576</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1523,10 +1520,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>9</v>
+        <v>20</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
       </c>
       <c r="D5" s="7">
         <v>45572</v>
@@ -1544,10 +1541,10 @@
         <v>45576</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1555,10 +1552,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>9</v>
+        <v>21</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
       </c>
       <c r="D6" s="7">
         <v>45572</v>
@@ -1576,10 +1573,10 @@
         <v>45576</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1587,10 +1584,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>9</v>
+        <v>22</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
       </c>
       <c r="D7" s="7">
         <v>45572</v>
@@ -1608,10 +1605,10 @@
         <v>45576</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1619,10 +1616,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>9</v>
+        <v>22</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
       </c>
       <c r="D8" s="7">
         <v>45572</v>
@@ -1640,10 +1637,10 @@
         <v>45576</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1651,10 +1648,10 @@
         <v>5</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>9</v>
+        <v>23</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
       </c>
       <c r="D9" s="7">
         <v>45572</v>
@@ -1672,10 +1669,10 @@
         <v>45576</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1683,10 +1680,10 @@
         <v>5</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>9</v>
+        <v>24</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
       </c>
       <c r="D10" s="7">
         <v>45572</v>
@@ -1704,10 +1701,10 @@
         <v>45576</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adicionando novos arquivos e atualizando relatórios
</commit_message>
<xml_diff>
--- a/Base/Backlog.xlsx
+++ b/Base/Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franciscoj\Python_Initial\Pyhton_Web\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4188468-5D14-4D95-97AC-E4F377FF4CA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2233FA6F-D616-4B18-8F8B-979A0D63742D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="418" xr2:uid="{89A3EF9E-2AF9-420D-85DF-9BB5B68F651F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="418" activeTab="1" xr2:uid="{89A3EF9E-2AF9-420D-85DF-9BB5B68F651F}"/>
   </bookViews>
   <sheets>
     <sheet name="SPN" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="24">
   <si>
     <t>Backlog</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>Ano</t>
+  </si>
+  <si>
+    <t>Resolvido</t>
   </si>
 </sst>
 </file>
@@ -547,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16A6A408-5BF6-4E16-8C71-EC6EB1F5A842}">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -701,7 +704,7 @@
         <v>45663</v>
       </c>
       <c r="J4" s="18" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K4" s="17" t="s">
         <v>17</v>
@@ -771,7 +774,7 @@
         <v>45663</v>
       </c>
       <c r="J6" s="18" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K6" s="17" t="s">
         <v>17</v>
@@ -1014,8 +1017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69362A46-9E44-40AB-81A2-018EE27C1DC6}">
   <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1099,7 +1102,7 @@
         <v>45663</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K2" s="13" t="s">
         <v>11</v>
@@ -1134,7 +1137,7 @@
         <v>45663</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K3" s="13" t="s">
         <v>11</v>
@@ -1169,7 +1172,7 @@
         <v>45663</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K4" s="13" t="s">
         <v>11</v>
@@ -1204,7 +1207,7 @@
         <v>45663</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K5" s="13" t="s">
         <v>11</v>

</xml_diff>